<commit_message>
Before adding the real time application
</commit_message>
<xml_diff>
--- a/static/app_data/produccion_energetica/produccion_energetica.xlsx
+++ b/static/app_data/produccion_energetica/produccion_energetica.xlsx
@@ -72,9 +72,6 @@
     <t>/cal/generation_now/hidraulica</t>
   </si>
   <si>
-    <t>/cal/generation_now/otra generacion</t>
-  </si>
-  <si>
     <t>/cal/generation_now/no convencional</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Térmica</t>
+  </si>
+  <si>
+    <t>/cal/generation_now/termoelectrica + interconnexion</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>rgba(166,166,166,1)</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -584,7 +584,7 @@
         <v>rgba(255,217,102,1)</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>rgba(169,208,142,1)</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forecasting electric demand vr.0.1
</commit_message>
<xml_diff>
--- a/static/app_data/produccion_energetica/produccion_energetica.xlsx
+++ b/static/app_data/produccion_energetica/produccion_energetica.xlsx
@@ -120,18 +120,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8989FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4FA7FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -139,6 +127,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5897DD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9803B1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,11 +177,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,6 +190,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9803B1"/>
+      <color rgb="FFE13EFC"/>
+      <color rgb="FF7D3DFD"/>
+      <color rgb="FF4D02E4"/>
+      <color rgb="FFA578FE"/>
+      <color rgb="FF5897DD"/>
       <color rgb="FF4FA7FF"/>
       <color rgb="FF8989FF"/>
     </mruColors>
@@ -487,7 +493,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,19 +505,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -543,9 +549,9 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="8" t="str">
         <f>[1]!getcolor(D3)</f>
-        <v>rgba(137,137,255,1)</v>
+        <v>rgba(152,3,177,1)</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -561,9 +567,9 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="str">
+      <c r="D4" s="7" t="str">
         <f>[1]!getcolor(D4)</f>
-        <v>rgba(79,167,255,1)</v>
+        <v>rgba(88,151,221,1)</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -579,7 +585,7 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="str">
+      <c r="D5" s="4" t="str">
         <f>[1]!getcolor(D5)</f>
         <v>rgba(255,217,102,1)</v>
       </c>
@@ -597,7 +603,7 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" s="5" t="str">
         <f>[1]!getcolor(D6)</f>
         <v>rgba(169,208,142,1)</v>
       </c>

</xml_diff>

<commit_message>
Despliegue nacional de distribución
</commit_message>
<xml_diff>
--- a/static/app_data/produccion_energetica/produccion_energetica.xlsx
+++ b/static/app_data/produccion_energetica/produccion_energetica.xlsx
@@ -69,26 +69,26 @@
     <t>/cal/exportation_energy_now</t>
   </si>
   <si>
-    <t>/cal/generation_now/hidraulica</t>
-  </si>
-  <si>
-    <t>/cal/generation_now/no convencional</t>
-  </si>
-  <si>
-    <t>/cal/generation_now/total</t>
-  </si>
-  <si>
     <t>Térmica</t>
   </si>
   <si>
-    <t>/cal/generation_now/termoelectrica + interconnexion</t>
+    <t>/cal/generation_now/Total</t>
+  </si>
+  <si>
+    <t>/cal/generation_now/No convencional</t>
+  </si>
+  <si>
+    <t>/cal/generation_now/Hidráulica</t>
+  </si>
+  <si>
+    <t>/cal/generation_now/Termoeléctrica + interconexión</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +100,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -182,6 +190,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +503,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +546,7 @@
         <v>rgba(166,166,166,1)</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -553,7 +563,7 @@
         <f>[1]!getcolor(D3)</f>
         <v>rgba(152,3,177,1)</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -572,7 +582,7 @@
         <v>rgba(88,151,221,1)</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -580,7 +590,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -589,7 +599,7 @@
         <f>[1]!getcolor(D5)</f>
         <v>rgba(255,217,102,1)</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -608,7 +618,7 @@
         <v>rgba(169,208,142,1)</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>